<commit_message>
trimming text on inventory
</commit_message>
<xml_diff>
--- a/data/QtekBOM.xlsx
+++ b/data/QtekBOM.xlsx
@@ -538,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -553,13 +553,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -789,7 +782,10 @@
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
@@ -829,31 +825,48 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="9" t="b">
+      <c r="F3" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="2">
@@ -865,21 +878,21 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>12</v>
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="9" t="b">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="2">
@@ -891,21 +904,21 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="9" t="b">
+        <v>21</v>
+      </c>
+      <c r="F5" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="2">
@@ -917,36 +930,36 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>4.0</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1.0</v>
-      </c>
       <c r="H6" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>22</v>
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>16</v>
@@ -955,13 +968,13 @@
         <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="9" t="b">
+        <v>26</v>
+      </c>
+      <c r="F7" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H7" s="2">
         <v>0.0</v>
@@ -969,10 +982,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>25</v>
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -981,9 +994,9 @@
         <v>23</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="9" t="b">
+        <v>28</v>
+      </c>
+      <c r="F8" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G8" s="2">
@@ -995,10 +1008,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>27</v>
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
@@ -1007,9 +1020,9 @@
         <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="9" t="b">
+        <v>30</v>
+      </c>
+      <c r="F9" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G9" s="2">
@@ -1021,36 +1034,36 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>29</v>
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="9" t="b">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="F10" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="G10" s="2">
         <v>1.0</v>
       </c>
       <c r="H10" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>31</v>
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>16</v>
@@ -1059,9 +1072,9 @@
         <v>32</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="9" t="b">
+        <v>35</v>
+      </c>
+      <c r="F11" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G11" s="2">
@@ -1073,10 +1086,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>34</v>
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
@@ -1085,9 +1098,9 @@
         <v>32</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="9" t="b">
+        <v>37</v>
+      </c>
+      <c r="F12" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G12" s="2">
@@ -1099,21 +1112,21 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>36</v>
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="9" t="b">
+        <v>40</v>
+      </c>
+      <c r="F13" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G13" s="2">
@@ -1125,21 +1138,21 @@
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>38</v>
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="9" t="b">
+        <v>42</v>
+      </c>
+      <c r="F14" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G14" s="2">
@@ -1151,10 +1164,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>41</v>
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
@@ -1163,9 +1176,9 @@
         <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="9" t="b">
+        <v>44</v>
+      </c>
+      <c r="F15" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G15" s="2">
@@ -1177,10 +1190,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>43</v>
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>13</v>
@@ -1189,9 +1202,9 @@
         <v>39</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="9" t="b">
+        <v>46</v>
+      </c>
+      <c r="F16" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G16" s="2">
@@ -1203,10 +1216,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>45</v>
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>13</v>
@@ -1215,24 +1228,24 @@
         <v>39</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="9" t="b">
+        <v>48</v>
+      </c>
+      <c r="F17" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G17" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H17" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>47</v>
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>13</v>
@@ -1241,24 +1254,24 @@
         <v>39</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="9" t="b">
+        <v>50</v>
+      </c>
+      <c r="F18" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G18" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H18" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>49</v>
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>13</v>
@@ -1267,9 +1280,9 @@
         <v>39</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="9" t="b">
+        <v>52</v>
+      </c>
+      <c r="F19" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G19" s="2">
@@ -1281,10 +1294,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>51</v>
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>13</v>
@@ -1293,49 +1306,49 @@
         <v>39</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="9" t="b">
+        <v>54</v>
+      </c>
+      <c r="F20" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G20" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H20" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>53</v>
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="9" t="b">
+        <v>56</v>
+      </c>
+      <c r="E21" s="3">
+        <v>3044102.0</v>
+      </c>
+      <c r="F21" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G21" s="2">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="H21" s="2">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="B22" s="8" t="s">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1345,24 +1358,24 @@
         <v>56</v>
       </c>
       <c r="E22" s="3">
-        <v>3044102.0</v>
-      </c>
-      <c r="F22" s="9" t="b">
+        <v>3044636.0</v>
+      </c>
+      <c r="F22" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G22" s="2">
-        <v>5.0</v>
+        <v>39.0</v>
       </c>
       <c r="H22" s="2">
-        <v>5.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>55</v>
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>16</v>
@@ -1371,23 +1384,23 @@
         <v>56</v>
       </c>
       <c r="E23" s="3">
-        <v>3044636.0</v>
-      </c>
-      <c r="F23" s="9" t="b">
+        <v>3047293.0</v>
+      </c>
+      <c r="F23" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G23" s="2">
-        <v>39.0</v>
+        <v>2.0</v>
       </c>
       <c r="H23" s="2">
-        <v>39.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="B24" s="8" t="s">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1397,24 +1410,24 @@
         <v>56</v>
       </c>
       <c r="E24" s="3">
-        <v>3047293.0</v>
-      </c>
-      <c r="F24" s="9" t="b">
+        <v>3047028.0</v>
+      </c>
+      <c r="F24" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G24" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H24" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <v>23.0</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>57</v>
+        <v>24.0</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>16</v>
@@ -1423,24 +1436,24 @@
         <v>56</v>
       </c>
       <c r="E25" s="3">
-        <v>3047028.0</v>
-      </c>
-      <c r="F25" s="9" t="b">
+        <v>3022276.0</v>
+      </c>
+      <c r="F25" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G25" s="2">
-        <v>1.0</v>
+        <v>16.0</v>
       </c>
       <c r="H25" s="2">
-        <v>1.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>58</v>
+        <v>25.0</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>16</v>
@@ -1449,24 +1462,24 @@
         <v>56</v>
       </c>
       <c r="E26" s="3">
-        <v>3022276.0</v>
-      </c>
-      <c r="F26" s="9" t="b">
+        <v>3030161.0</v>
+      </c>
+      <c r="F26" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G26" s="2">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
       <c r="H26" s="2">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>59</v>
+        <v>26.0</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>16</v>
@@ -1475,9 +1488,9 @@
         <v>56</v>
       </c>
       <c r="E27" s="3">
-        <v>3030161.0</v>
-      </c>
-      <c r="F27" s="9" t="b">
+        <v>3030213.0</v>
+      </c>
+      <c r="F27" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G27" s="2">
@@ -1489,10 +1502,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>60</v>
+        <v>27.0</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>16</v>
@@ -1501,9 +1514,9 @@
         <v>56</v>
       </c>
       <c r="E28" s="3">
-        <v>3030213.0</v>
-      </c>
-      <c r="F28" s="9" t="b">
+        <v>3036877.0</v>
+      </c>
+      <c r="F28" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G28" s="2">
@@ -1515,10 +1528,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>61</v>
+        <v>28.0</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>16</v>
@@ -1527,87 +1540,87 @@
         <v>56</v>
       </c>
       <c r="E29" s="3">
-        <v>3036877.0</v>
-      </c>
-      <c r="F29" s="9" t="b">
+        <v>2866310.0</v>
+      </c>
+      <c r="F29" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G29" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H29" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1">
-        <v>28.0</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>62</v>
+        <v>29.0</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="3">
-        <v>2866310.0</v>
-      </c>
-      <c r="F30" s="9" t="b">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G30" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H30" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>63</v>
+        <v>30.0</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="9" t="b">
-        <v>0</v>
+        <v>66</v>
+      </c>
+      <c r="F31" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="G31" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H31" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>65</v>
+        <v>31.0</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="9" t="b">
+        <v>68</v>
+      </c>
+      <c r="F32" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G32" s="2">
@@ -1619,21 +1632,21 @@
     </row>
     <row r="33">
       <c r="A33" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>67</v>
+        <v>32.0</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="9" t="b">
+        <v>56</v>
+      </c>
+      <c r="E33" s="3">
+        <v>801733.0</v>
+      </c>
+      <c r="F33" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G33" s="2">
@@ -1645,21 +1658,21 @@
     </row>
     <row r="34">
       <c r="A34" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>69</v>
+        <v>33.0</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="3">
-        <v>801733.0</v>
-      </c>
-      <c r="F34" s="9" t="b">
+      <c r="E34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G34" s="2">
@@ -1671,21 +1684,21 @@
     </row>
     <row r="35">
       <c r="A35" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>70</v>
+        <v>34.0</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F35" s="9" t="b">
+        <v>74</v>
+      </c>
+      <c r="F35" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G35" s="2">
@@ -1697,21 +1710,21 @@
     </row>
     <row r="36">
       <c r="A36" s="1">
-        <v>34.0</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>72</v>
+        <v>35.0</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" s="9" t="b">
+        <v>76</v>
+      </c>
+      <c r="F36" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G36" s="2">
@@ -1723,10 +1736,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1">
-        <v>35.0</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>75</v>
+        <v>36.0</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>16</v>
@@ -1735,24 +1748,24 @@
         <v>39</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F37" s="9" t="b">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="F37" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G37" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H37" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>77</v>
+        <v>37.0</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>16</v>
@@ -1761,9 +1774,9 @@
         <v>39</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F38" s="9" t="b">
+        <v>80</v>
+      </c>
+      <c r="F38" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G38" s="2">
@@ -1775,47 +1788,47 @@
     </row>
     <row r="39">
       <c r="A39" s="1">
-        <v>37.0</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>79</v>
+        <v>38.0</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="9" t="b">
+        <v>83</v>
+      </c>
+      <c r="F39" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G39" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H39" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1">
-        <v>38.0</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>81</v>
+        <v>39.0</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F40" s="9" t="b">
+        <v>85</v>
+      </c>
+      <c r="F40" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G40" s="2">
@@ -1827,21 +1840,21 @@
     </row>
     <row r="41">
       <c r="A41" s="1">
-        <v>39.0</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>84</v>
+        <v>40.0</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F41" s="9" t="b">
+        <v>56</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1085039.0</v>
+      </c>
+      <c r="F41" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G41" s="2">
@@ -1853,73 +1866,73 @@
     </row>
     <row r="42">
       <c r="A42" s="1">
-        <v>40.0</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>86</v>
+        <v>41.0</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42" s="3">
-        <v>1085039.0</v>
-      </c>
-      <c r="F42" s="9" t="b">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G42" s="2">
         <v>1.0</v>
       </c>
       <c r="H42" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1">
-        <v>41.0</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>87</v>
+        <v>42.0</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F43" s="9" t="b">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="F43" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="G43" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H43" s="2">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1">
-        <v>42.0</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>89</v>
+        <v>43.0</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F44" s="9" t="b">
+        <v>92</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G44" s="2">
@@ -1931,62 +1944,62 @@
     </row>
     <row r="45">
       <c r="A45" s="1">
-        <v>43.0</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>91</v>
+        <v>44.0</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45" s="9" t="b">
+      <c r="E45" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G45" s="2">
-        <v>2.0</v>
+        <v>30.0</v>
       </c>
       <c r="H45" s="2">
-        <v>2.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1">
-        <v>44.0</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>93</v>
+        <v>45.0</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>94</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" s="9" t="b">
+        <v>56</v>
+      </c>
+      <c r="E46" s="8">
+        <v>1681389.0</v>
+      </c>
+      <c r="F46" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G46" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H46" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1">
-        <v>45.0</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>96</v>
+        <v>46.0</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>94</v>
@@ -1994,25 +2007,25 @@
       <c r="D47" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E47" s="11">
-        <v>1681389.0</v>
-      </c>
-      <c r="F47" s="9" t="b">
+      <c r="E47" s="8">
+        <v>1668247.0</v>
+      </c>
+      <c r="F47" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G47" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H47" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1">
-        <v>46.0</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>97</v>
+        <v>47.0</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>94</v>
@@ -2020,25 +2033,25 @@
       <c r="D48" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E48" s="11">
-        <v>1668247.0</v>
-      </c>
-      <c r="F48" s="9" t="b">
+      <c r="E48" s="8">
+        <v>1669848.0</v>
+      </c>
+      <c r="F48" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G48" s="2">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H48" s="2">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1">
-        <v>47.0</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>98</v>
+        <v>48.0</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>94</v>
@@ -2046,25 +2059,25 @@
       <c r="D49" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="11">
-        <v>1669848.0</v>
-      </c>
-      <c r="F49" s="9" t="b">
+      <c r="E49" s="8">
+        <v>1668124.0</v>
+      </c>
+      <c r="F49" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G49" s="2">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H49" s="2">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1">
-        <v>48.0</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>99</v>
+        <v>49.0</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>94</v>
@@ -2072,36 +2085,36 @@
       <c r="D50" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="11">
-        <v>1668124.0</v>
-      </c>
-      <c r="F50" s="9" t="b">
-        <v>1</v>
+      <c r="E50" s="8">
+        <v>1669628.0</v>
+      </c>
+      <c r="F50" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G50" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H50" s="2">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1">
-        <v>49.0</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>100</v>
+        <v>50.0</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E51" s="11">
-        <v>1669628.0</v>
-      </c>
-      <c r="F51" s="9" t="b">
+      <c r="D51" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F51" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G51" s="2">
@@ -2113,21 +2126,21 @@
     </row>
     <row r="52">
       <c r="A52" s="1">
-        <v>50.0</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>101</v>
+        <v>51.0</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D52" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="F52" s="9" t="b">
+      <c r="D52" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E52" s="8">
+        <v>1415943.0</v>
+      </c>
+      <c r="F52" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G52" s="2">
@@ -2139,47 +2152,47 @@
     </row>
     <row r="53">
       <c r="A53" s="1">
-        <v>51.0</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>104</v>
+        <v>52.0</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>94</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E53" s="11">
-        <v>1415943.0</v>
-      </c>
-      <c r="F53" s="9" t="b">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="G53" s="2">
         <v>1.0</v>
       </c>
       <c r="H53" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1">
-        <v>52.0</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>105</v>
+        <v>53.0</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>94</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F54" s="9" t="b">
+        <v>56</v>
+      </c>
+      <c r="E54" s="8">
+        <v>1683002.0</v>
+      </c>
+      <c r="F54" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G54" s="2">
@@ -2191,21 +2204,21 @@
     </row>
     <row r="55">
       <c r="A55" s="1">
-        <v>53.0</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>107</v>
+        <v>54.0</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E55" s="11">
-        <v>1683002.0</v>
-      </c>
-      <c r="F55" s="9" t="b">
+      <c r="D55" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G55" s="2">
@@ -2217,21 +2230,21 @@
     </row>
     <row r="56">
       <c r="A56" s="1">
-        <v>54.0</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>108</v>
+        <v>55.0</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D56" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="F56" s="9" t="b">
+      <c r="D56" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F56" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G56" s="2">
@@ -2243,47 +2256,47 @@
     </row>
     <row r="57">
       <c r="A57" s="1">
-        <v>55.0</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>111</v>
+        <v>56.0</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D57" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="F57" s="9" t="b">
-        <v>1</v>
+      <c r="D57" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E57" s="8">
+        <v>1520372.0</v>
+      </c>
+      <c r="F57" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G57" s="2">
         <v>1.0</v>
       </c>
       <c r="H57" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1">
-        <v>56.0</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>113</v>
+        <v>57.0</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E58" s="11">
-        <v>1520372.0</v>
-      </c>
-      <c r="F58" s="9" t="b">
+        <v>115</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F58" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G58" s="2">
@@ -2295,10 +2308,10 @@
     </row>
     <row r="59">
       <c r="A59" s="1">
-        <v>57.0</v>
+        <v>58.0</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>16</v>
@@ -2309,7 +2322,7 @@
       <c r="E59" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F59" s="9" t="b">
+      <c r="F59" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G59" s="2">
@@ -2321,13 +2334,13 @@
     </row>
     <row r="60">
       <c r="A60" s="1">
-        <v>58.0</v>
+        <v>59.0</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>116</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>115</v>
@@ -2335,33 +2348,33 @@
       <c r="E60" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F60" s="9" t="b">
-        <v>0</v>
+      <c r="F60" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="G60" s="2">
         <v>1.0</v>
       </c>
       <c r="H60" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1">
-        <v>59.0</v>
+        <v>60.0</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F61" s="9" t="b">
+        <v>120</v>
+      </c>
+      <c r="F61" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G61" s="2">
@@ -2373,21 +2386,21 @@
     </row>
     <row r="62">
       <c r="A62" s="1">
-        <v>60.0</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>118</v>
+        <v>61.0</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F62" s="9" t="b">
+        <v>39</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F62" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G62" s="2">
@@ -2399,10 +2412,10 @@
     </row>
     <row r="63">
       <c r="A63" s="1">
-        <v>61.0</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>41</v>
+        <v>62.0</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>117</v>
@@ -2410,10 +2423,10 @@
       <c r="D63" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F63" s="9" t="b">
+      <c r="E63" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F63" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G63" s="2">
@@ -2425,10 +2438,10 @@
     </row>
     <row r="64">
       <c r="A64" s="1">
-        <v>62.0</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>51</v>
+        <v>63.0</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>117</v>
@@ -2437,9 +2450,9 @@
         <v>39</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F64" s="9" t="b">
+        <v>122</v>
+      </c>
+      <c r="F64" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G64" s="2">
@@ -2451,21 +2464,21 @@
     </row>
     <row r="65">
       <c r="A65" s="1">
-        <v>63.0</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>41</v>
+        <v>64.0</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F65" s="9" t="b">
+        <v>124</v>
+      </c>
+      <c r="F65" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G65" s="2">
@@ -2477,10 +2490,10 @@
     </row>
     <row r="66">
       <c r="A66" s="1">
-        <v>64.0</v>
+        <v>65.0</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>117</v>
@@ -2489,9 +2502,9 @@
         <v>102</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F66" s="9" t="b">
+        <v>126</v>
+      </c>
+      <c r="F66" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G66" s="2">
@@ -2503,21 +2516,21 @@
     </row>
     <row r="67">
       <c r="A67" s="1">
-        <v>65.0</v>
+        <v>66.0</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F67" s="9" t="b">
+        <v>128</v>
+      </c>
+      <c r="F67" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G67" s="2">
@@ -2529,21 +2542,21 @@
     </row>
     <row r="68">
       <c r="A68" s="1">
-        <v>66.0</v>
+        <v>67.0</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F68" s="9" t="b">
+        <v>131</v>
+      </c>
+      <c r="F68" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G68" s="2">
@@ -2555,36 +2568,36 @@
     </row>
     <row r="69">
       <c r="A69" s="1">
-        <v>67.0</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>129</v>
+        <v>68.0</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F69" s="9" t="b">
+        <v>39</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F69" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G69" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H69" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1">
-        <v>68.0</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>53</v>
+        <v>69.0</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>117</v>
@@ -2593,24 +2606,24 @@
         <v>39</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F70" s="9" t="b">
+        <v>133</v>
+      </c>
+      <c r="F70" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G70" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H70" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1">
-        <v>69.0</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>132</v>
+        <v>70.0</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>117</v>
@@ -2619,9 +2632,9 @@
         <v>39</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F71" s="9" t="b">
+        <v>44</v>
+      </c>
+      <c r="F71" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G71" s="2">
@@ -2633,10 +2646,10 @@
     </row>
     <row r="72">
       <c r="A72" s="1">
-        <v>70.0</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>43</v>
+        <v>71.0</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>117</v>
@@ -2645,24 +2658,24 @@
         <v>39</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F72" s="9" t="b">
+        <v>46</v>
+      </c>
+      <c r="F72" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G72" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H72" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1">
-        <v>71.0</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>45</v>
+        <v>72.0</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>117</v>
@@ -2671,9 +2684,9 @@
         <v>39</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F73" s="9" t="b">
+        <v>48</v>
+      </c>
+      <c r="F73" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G73" s="2">
@@ -2685,36 +2698,36 @@
     </row>
     <row r="74">
       <c r="A74" s="1">
-        <v>72.0</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>47</v>
+        <v>73.0</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F74" s="9" t="b">
+        <v>135</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F74" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G74" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H74" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1">
-        <v>73.0</v>
+        <v>74.0</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>117</v>
@@ -2723,9 +2736,9 @@
         <v>135</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F75" s="9" t="b">
+        <v>138</v>
+      </c>
+      <c r="F75" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G75" s="2">
@@ -2737,10 +2750,10 @@
     </row>
     <row r="76">
       <c r="A76" s="1">
-        <v>74.0</v>
+        <v>75.0</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>117</v>
@@ -2749,9 +2762,9 @@
         <v>135</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F76" s="9" t="b">
+        <v>140</v>
+      </c>
+      <c r="F76" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G76" s="2">
@@ -2763,21 +2776,21 @@
     </row>
     <row r="77">
       <c r="A77" s="1">
-        <v>75.0</v>
+        <v>76.0</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>117</v>
+        <v>13</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F77" s="9" t="b">
+        <v>142</v>
+      </c>
+      <c r="F77" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G77" s="2">
@@ -2789,10 +2802,10 @@
     </row>
     <row r="78">
       <c r="A78" s="1">
-        <v>76.0</v>
+        <v>77.0</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>13</v>
@@ -2801,9 +2814,9 @@
         <v>135</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F78" s="9" t="b">
+        <v>144</v>
+      </c>
+      <c r="F78" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G78" s="2">
@@ -2815,10 +2828,10 @@
     </row>
     <row r="79">
       <c r="A79" s="1">
-        <v>77.0</v>
+        <v>78.0</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>13</v>
@@ -2827,9 +2840,9 @@
         <v>135</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F79" s="9" t="b">
+        <v>146</v>
+      </c>
+      <c r="F79" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G79" s="2">
@@ -2841,21 +2854,21 @@
     </row>
     <row r="80">
       <c r="A80" s="1">
-        <v>78.0</v>
+        <v>79.0</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F80" s="9" t="b">
+        <v>148</v>
+      </c>
+      <c r="F80" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G80" s="2">
@@ -2867,10 +2880,10 @@
     </row>
     <row r="81">
       <c r="A81" s="1">
-        <v>79.0</v>
+        <v>80.0</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>9</v>
@@ -2879,10 +2892,10 @@
         <v>135</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F81" s="9" t="b">
-        <v>1</v>
+        <v>150</v>
+      </c>
+      <c r="F81" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G81" s="2">
         <v>1.0</v>
@@ -2893,10 +2906,10 @@
     </row>
     <row r="82">
       <c r="A82" s="1">
-        <v>80.0</v>
+        <v>81.0</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>9</v>
@@ -2905,9 +2918,9 @@
         <v>135</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F82" s="9" t="b">
+        <v>152</v>
+      </c>
+      <c r="F82" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G82" s="2">
@@ -2919,10 +2932,10 @@
     </row>
     <row r="83">
       <c r="A83" s="1">
-        <v>81.0</v>
+        <v>82.0</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>9</v>
@@ -2931,10 +2944,10 @@
         <v>135</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F83" s="9" t="b">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="F83" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G83" s="2">
         <v>1.0</v>
@@ -2945,10 +2958,10 @@
     </row>
     <row r="84">
       <c r="A84" s="1">
-        <v>82.0</v>
+        <v>83.0</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>9</v>
@@ -2957,41 +2970,15 @@
         <v>135</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F84" s="9" t="b">
+        <v>156</v>
+      </c>
+      <c r="F84" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G84" s="2">
         <v>1.0</v>
       </c>
       <c r="H84" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1">
-        <v>83.0</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F85" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G85" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="H85" s="2">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished inventory page xlxs connections
</commit_message>
<xml_diff>
--- a/data/QtekBOM.xlsx
+++ b/data/QtekBOM.xlsx
@@ -37,6 +37,345 @@
     <t>Qty on hand</t>
   </si>
   <si>
+    <t>Breaker - 25A main disconnect</t>
+  </si>
+  <si>
+    <t>backplate</t>
+  </si>
+  <si>
+    <t>ABB</t>
+  </si>
+  <si>
+    <t>OT25F3</t>
+  </si>
+  <si>
+    <t>KBPC DRIVE</t>
+  </si>
+  <si>
+    <t>Penta</t>
+  </si>
+  <si>
+    <t>KBRC-24OD</t>
+  </si>
+  <si>
+    <t>Breaker - 1A</t>
+  </si>
+  <si>
+    <t>Schnieder</t>
+  </si>
+  <si>
+    <t>M9F42101</t>
+  </si>
+  <si>
+    <t>Breaker - 2A</t>
+  </si>
+  <si>
+    <t>M9F42102</t>
+  </si>
+  <si>
+    <t>Breaker - 15A</t>
+  </si>
+  <si>
+    <t>M9F42115</t>
+  </si>
+  <si>
+    <t>Breaker - 4A</t>
+  </si>
+  <si>
+    <t>M9F42104</t>
+  </si>
+  <si>
+    <t>Wireduct 1X3</t>
+  </si>
+  <si>
+    <t>Panduit</t>
+  </si>
+  <si>
+    <t>F1x3Lg6</t>
+  </si>
+  <si>
+    <t>Wireduct 1.5X3</t>
+  </si>
+  <si>
+    <t>F1.5x3Lg</t>
+  </si>
+  <si>
+    <t>Wireduct 2X3</t>
+  </si>
+  <si>
+    <t>F2x3Lg</t>
+  </si>
+  <si>
+    <t>Micro830 PLC controller</t>
+  </si>
+  <si>
+    <t>Allen Bradley</t>
+  </si>
+  <si>
+    <t>2080-LC50E-48QWB</t>
+  </si>
+  <si>
+    <t>Terminals</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Terminal endplate</t>
+  </si>
+  <si>
+    <t>Terminal endstop</t>
+  </si>
+  <si>
+    <t>Jumper 2 pole red</t>
+  </si>
+  <si>
+    <t>Jumper 10 pole</t>
+  </si>
+  <si>
+    <t>Jumper 2 pole blue</t>
+  </si>
+  <si>
+    <t>Power Supply 24VDC 5A</t>
+  </si>
+  <si>
+    <t>Contactor 24VDC</t>
+  </si>
+  <si>
+    <t>100-C16EJ01</t>
+  </si>
+  <si>
+    <t>Disconnect shaft</t>
+  </si>
+  <si>
+    <t>OXP6X290</t>
+  </si>
+  <si>
+    <t>Din rail</t>
+  </si>
+  <si>
+    <t>Safety relay</t>
+  </si>
+  <si>
+    <t>44OR-N23114</t>
+  </si>
+  <si>
+    <t>Control relay</t>
+  </si>
+  <si>
+    <t>700-HA33Z24-3-4</t>
+  </si>
+  <si>
+    <t>Control relay base</t>
+  </si>
+  <si>
+    <t>700-HN101</t>
+  </si>
+  <si>
+    <t>Control relay SPDT</t>
+  </si>
+  <si>
+    <t>700-HLT1Z24</t>
+  </si>
+  <si>
+    <t>Ethernet Switch</t>
+  </si>
+  <si>
+    <t>Diffuse Sensor</t>
+  </si>
+  <si>
+    <t>Baumer</t>
+  </si>
+  <si>
+    <t>OT500.GL-PLPLB.72F</t>
+  </si>
+  <si>
+    <t>Bushings for drive</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Ethernet cable 3ft</t>
+  </si>
+  <si>
+    <t>Startek</t>
+  </si>
+  <si>
+    <t>Ethernet cable 2ft</t>
+  </si>
+  <si>
+    <t>14 guage 3C</t>
+  </si>
+  <si>
+    <t>cables</t>
+  </si>
+  <si>
+    <t>3C-14</t>
+  </si>
+  <si>
+    <t>4pin M12 10M 90</t>
+  </si>
+  <si>
+    <t>4pin M12 5M 90</t>
+  </si>
+  <si>
+    <t>5pin M12 5M STR</t>
+  </si>
+  <si>
+    <t>4pin M12 5M STR</t>
+  </si>
+  <si>
+    <t>3pin M8 5M STR</t>
+  </si>
+  <si>
+    <t>3pin Valve cable PO Check Valve</t>
+  </si>
+  <si>
+    <t>MURR</t>
+  </si>
+  <si>
+    <t>7000-11081-6160500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3pin Valve cable </t>
+  </si>
+  <si>
+    <t>9pin Valvebank cable Female</t>
+  </si>
+  <si>
+    <t>889N-F9AF-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4pin M12 10M STR </t>
+  </si>
+  <si>
+    <t>12pin Micro 10M STR</t>
+  </si>
+  <si>
+    <t>MENCOM</t>
+  </si>
+  <si>
+    <t>MDCM-12MFP-10-B</t>
+  </si>
+  <si>
+    <t>RJ45 10M STR Female</t>
+  </si>
+  <si>
+    <t>7000-44711-7961000</t>
+  </si>
+  <si>
+    <t>8pin M12 10M STR</t>
+  </si>
+  <si>
+    <t>Backplate</t>
+  </si>
+  <si>
+    <t>enclosure</t>
+  </si>
+  <si>
+    <t>Klassen</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>Pushbutton Green</t>
+  </si>
+  <si>
+    <t>800FB-LF3</t>
+  </si>
+  <si>
+    <t>Pushbutton LED white</t>
+  </si>
+  <si>
+    <t>800FP-N3W</t>
+  </si>
+  <si>
+    <t>Pushbutton contact blocks NO</t>
+  </si>
+  <si>
+    <t>800F-X10</t>
+  </si>
+  <si>
+    <t>Pushbutton contact blocks NC</t>
+  </si>
+  <si>
+    <t>800F-X01</t>
+  </si>
+  <si>
+    <t>Keyed Selector Switch</t>
+  </si>
+  <si>
+    <t>800FP-KM22</t>
+  </si>
+  <si>
+    <t>Pushbutton ESTOP</t>
+  </si>
+  <si>
+    <t>800FP-MT64</t>
+  </si>
+  <si>
+    <t>Pushbutton latch</t>
+  </si>
+  <si>
+    <t>800FP-ALP</t>
+  </si>
+  <si>
+    <t>Disconnect handle</t>
+  </si>
+  <si>
+    <t>OHB45J6</t>
+  </si>
+  <si>
+    <t>Pilot Light Green</t>
+  </si>
+  <si>
+    <t>800FP-P3</t>
+  </si>
+  <si>
+    <t>RJ45 Bulkhead coupler</t>
+  </si>
+  <si>
+    <t>Graceport</t>
+  </si>
+  <si>
+    <t>N206-BC01-1ND</t>
+  </si>
+  <si>
+    <t>Digital Counter</t>
+  </si>
+  <si>
+    <t>IsI30.013AA01</t>
+  </si>
+  <si>
+    <t>Auxiliary contact 1 NO 1 NC</t>
+  </si>
+  <si>
+    <t>100-FA11</t>
+  </si>
+  <si>
+    <t>Lamacoid Status</t>
+  </si>
+  <si>
+    <t>ACP</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Lamacoid Hand Auto</t>
+  </si>
+  <si>
+    <t>handauto</t>
+  </si>
+  <si>
+    <t>Lamacoid ESTOP large</t>
+  </si>
+  <si>
+    <t>estoplarge</t>
+  </si>
+  <si>
     <t>Nema 12 Enclosure</t>
   </si>
   <si>
@@ -46,322 +385,34 @@
     <t>Klassenss</t>
   </si>
   <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>Backplate</t>
-  </si>
-  <si>
-    <t>enclosure</t>
-  </si>
-  <si>
-    <t>Klassen</t>
-  </si>
-  <si>
-    <t>Breaker - 25A main disconnect</t>
-  </si>
-  <si>
-    <t>backplate</t>
-  </si>
-  <si>
-    <t>ABB</t>
-  </si>
-  <si>
-    <t>OT25F3</t>
-  </si>
-  <si>
-    <t>KBPC DRIVE</t>
-  </si>
-  <si>
-    <t>Penta</t>
-  </si>
-  <si>
-    <t>KBRC-24OD</t>
-  </si>
-  <si>
-    <t>Breaker - 1A</t>
-  </si>
-  <si>
-    <t>Schnieder</t>
-  </si>
-  <si>
-    <t>M9F42101</t>
-  </si>
-  <si>
-    <t>Breaker - 2A</t>
-  </si>
-  <si>
-    <t>M9F42102</t>
-  </si>
-  <si>
-    <t>Breaker - 15A</t>
-  </si>
-  <si>
-    <t>M9F42115</t>
-  </si>
-  <si>
-    <t>Breaker - 4A</t>
-  </si>
-  <si>
-    <t>M9F42104</t>
-  </si>
-  <si>
-    <t>Wireduct 1X3</t>
-  </si>
-  <si>
-    <t>Panduit</t>
-  </si>
-  <si>
-    <t>F1x3Lg6</t>
-  </si>
-  <si>
-    <t>Wireduct 1.5X3</t>
-  </si>
-  <si>
-    <t>F1.5x3Lg</t>
-  </si>
-  <si>
-    <t>Wireduct 2X3</t>
-  </si>
-  <si>
-    <t>F2x3Lg</t>
-  </si>
-  <si>
-    <t>Micro830 PLC controller</t>
-  </si>
-  <si>
-    <t>Allen Bradley</t>
-  </si>
-  <si>
-    <t>2080-LC50E-48QWB</t>
-  </si>
-  <si>
-    <t>Pushbutton Green</t>
-  </si>
-  <si>
-    <t>800FB-LF3</t>
-  </si>
-  <si>
-    <t>Pushbutton LED white</t>
-  </si>
-  <si>
-    <t>800FP-N3W</t>
-  </si>
-  <si>
-    <t>Pushbutton contact blocks NO</t>
-  </si>
-  <si>
-    <t>800F-X10</t>
-  </si>
-  <si>
-    <t>Pushbutton contact blocks NC</t>
-  </si>
-  <si>
-    <t>800F-X01</t>
-  </si>
-  <si>
-    <t>Keyed Selector Switch</t>
-  </si>
-  <si>
-    <t>800FP-KM22</t>
-  </si>
-  <si>
-    <t>Pushbutton ESTOP</t>
-  </si>
-  <si>
-    <t>800FP-MT64</t>
-  </si>
-  <si>
-    <t>Pushbutton latch</t>
-  </si>
-  <si>
-    <t>800FP-ALP</t>
-  </si>
-  <si>
-    <t>Terminal</t>
-  </si>
-  <si>
-    <t>Phoenix</t>
-  </si>
-  <si>
-    <t>Terminal endplate</t>
-  </si>
-  <si>
-    <t>Terminal endstop</t>
-  </si>
-  <si>
-    <t>Jumper 2 pole red</t>
-  </si>
-  <si>
-    <t>Jumper 10 pole</t>
-  </si>
-  <si>
-    <t>Jumper 2 pole blue</t>
-  </si>
-  <si>
-    <t>Power Supply 24VDC 5A</t>
-  </si>
-  <si>
-    <t>Contactor 24VDC</t>
-  </si>
-  <si>
-    <t>100-C16EJ01</t>
-  </si>
-  <si>
-    <t>Disconnect handle</t>
-  </si>
-  <si>
-    <t>OHB45J6</t>
-  </si>
-  <si>
-    <t>Disconnect shaft</t>
-  </si>
-  <si>
-    <t>OXP6X290</t>
-  </si>
-  <si>
-    <t>Din rail</t>
-  </si>
-  <si>
-    <t>Pilot Light Green</t>
-  </si>
-  <si>
-    <t>800FP-P3</t>
-  </si>
-  <si>
-    <t>RJ45 Bulkhead coupler</t>
-  </si>
-  <si>
-    <t>Graceport</t>
-  </si>
-  <si>
-    <t>N206-BC01-1ND</t>
-  </si>
-  <si>
-    <t>Safety relay</t>
-  </si>
-  <si>
-    <t>44OR-N23114</t>
-  </si>
-  <si>
-    <t>Control relay</t>
-  </si>
-  <si>
-    <t>700-HA33Z24-3-4</t>
-  </si>
-  <si>
-    <t>Control relay base</t>
-  </si>
-  <si>
-    <t>700-HN101</t>
-  </si>
-  <si>
-    <t>Digital Counter</t>
-  </si>
-  <si>
-    <t>Baumer</t>
-  </si>
-  <si>
-    <t>IsI30.013AA01</t>
-  </si>
-  <si>
-    <t>Control relay SPDT</t>
-  </si>
-  <si>
-    <t>700-HLT1Z24</t>
-  </si>
-  <si>
-    <t>Ethernet Switch</t>
-  </si>
-  <si>
-    <t>Diffuse Sensor</t>
-  </si>
-  <si>
-    <t>OT500.GL-PLPLB.72F</t>
-  </si>
-  <si>
-    <t>Auxiliary contact 1 NO 1 NC</t>
-  </si>
-  <si>
-    <t>100-FA11</t>
-  </si>
-  <si>
-    <t>Bushings for drive</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>14 guage 3C</t>
-  </si>
-  <si>
-    <t>cables</t>
-  </si>
-  <si>
-    <t>3C-14</t>
-  </si>
-  <si>
-    <t>4pin M12 10M 90</t>
-  </si>
-  <si>
-    <t>4pin M12 5M 90</t>
-  </si>
-  <si>
-    <t>5pin M12 5M STR</t>
-  </si>
-  <si>
-    <t>4pin M12 5M STR</t>
-  </si>
-  <si>
-    <t>3pin M8 5M STR</t>
-  </si>
-  <si>
-    <t>3pin Valve cable PO Check Valve</t>
-  </si>
-  <si>
-    <t>MURR</t>
-  </si>
-  <si>
-    <t>7000-11081-6160500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3pin Valve cable </t>
-  </si>
-  <si>
-    <t>9pin Valvebank cable Female</t>
-  </si>
-  <si>
-    <t>889N-F9AF-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4pin M12 10M STR </t>
-  </si>
-  <si>
-    <t>12pin Micro 10M STR</t>
-  </si>
-  <si>
-    <t>MENCOM</t>
-  </si>
-  <si>
-    <t>MDCM-12MFP-10-B</t>
-  </si>
-  <si>
-    <t>RJ45 10M STR Female</t>
-  </si>
-  <si>
-    <t>7000-44711-7961000</t>
-  </si>
-  <si>
-    <t>8pin M12 10M STR</t>
-  </si>
-  <si>
-    <t>Ethernet cable 3ft</t>
-  </si>
-  <si>
-    <t>Startek</t>
-  </si>
-  <si>
-    <t>Ethernet cable 2ft</t>
+    <t>Brady Labels backplate</t>
+  </si>
+  <si>
+    <t>bradylabels</t>
+  </si>
+  <si>
+    <t>Wire labels backplate</t>
+  </si>
+  <si>
+    <t>WL-backplate</t>
+  </si>
+  <si>
+    <t>Wire labels door</t>
+  </si>
+  <si>
+    <t>WL-door</t>
+  </si>
+  <si>
+    <t>Wire labels OP Station</t>
+  </si>
+  <si>
+    <t>WL-OP</t>
+  </si>
+  <si>
+    <t>Wire labels cables</t>
+  </si>
+  <si>
+    <t>WL--cables</t>
   </si>
   <si>
     <t>op stn</t>
@@ -418,9 +469,6 @@
     <t>Lamacoid ESTOP small</t>
   </si>
   <si>
-    <t>ACP</t>
-  </si>
-  <si>
     <t>estopsmall</t>
   </si>
   <si>
@@ -434,54 +482,6 @@
   </si>
   <si>
     <t>clamps</t>
-  </si>
-  <si>
-    <t>Lamacoid Status</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>Lamacoid Hand Auto</t>
-  </si>
-  <si>
-    <t>handauto</t>
-  </si>
-  <si>
-    <t>Lamacoid ESTOP large</t>
-  </si>
-  <si>
-    <t>estoplarge</t>
-  </si>
-  <si>
-    <t>Brady Labels backplate</t>
-  </si>
-  <si>
-    <t>bradylabels</t>
-  </si>
-  <si>
-    <t>Wire labels backplate</t>
-  </si>
-  <si>
-    <t>WL-backplate</t>
-  </si>
-  <si>
-    <t>Wire labels door</t>
-  </si>
-  <si>
-    <t>WL-door</t>
-  </si>
-  <si>
-    <t>Wire labels OP Station</t>
-  </si>
-  <si>
-    <t>WL-OP</t>
-  </si>
-  <si>
-    <t>Wire labels cables</t>
-  </si>
-  <si>
-    <t>WL--cables</t>
   </si>
 </sst>
 </file>
@@ -826,7 +826,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
@@ -852,19 +852,19 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F3" s="6" t="b">
         <v>1</v>
@@ -878,77 +878,77 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F4" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H4" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2">
         <v>1.0</v>
       </c>
       <c r="H5" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="2">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H6" s="2">
         <v>0.0</v>
@@ -956,19 +956,19 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F7" s="6" t="b">
         <v>0</v>
@@ -982,71 +982,71 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2">
         <v>1.0</v>
       </c>
       <c r="H8" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2">
         <v>1.0</v>
       </c>
       <c r="H9" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" s="6" t="b">
         <v>1</v>
@@ -1060,19 +1060,19 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F11" s="6" t="b">
         <v>1</v>
@@ -1086,97 +1086,97 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>11.0</v>
+        <v>20.0</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3044102.0</v>
       </c>
       <c r="F12" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G12" s="2">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H12" s="2">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>12.0</v>
+        <v>21.0</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3044636.0</v>
       </c>
       <c r="F13" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G13" s="2">
-        <v>1.0</v>
+        <v>39.0</v>
       </c>
       <c r="H13" s="2">
-        <v>1.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>13.0</v>
+        <v>22.0</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3047293.0</v>
       </c>
       <c r="F14" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G14" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H14" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>14.0</v>
+        <v>23.0</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="E15" s="3">
+        <v>3047028.0</v>
       </c>
       <c r="F15" s="6" t="b">
         <v>1</v>
@@ -1190,227 +1190,227 @@
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>15.0</v>
+        <v>24.0</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3022276.0</v>
       </c>
       <c r="F16" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G16" s="2">
-        <v>1.0</v>
+        <v>16.0</v>
       </c>
       <c r="H16" s="2">
-        <v>1.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>16.0</v>
+        <v>25.0</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3030161.0</v>
       </c>
       <c r="F17" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G17" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H17" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>17.0</v>
+        <v>26.0</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>50</v>
+        <v>35</v>
+      </c>
+      <c r="E18" s="3">
+        <v>3030213.0</v>
       </c>
       <c r="F18" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G18" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H18" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>18.0</v>
+        <v>27.0</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>52</v>
+        <v>35</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3036877.0</v>
       </c>
       <c r="F19" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G19" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H19" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>19.0</v>
+        <v>28.0</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>54</v>
+        <v>35</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2866310.0</v>
       </c>
       <c r="F20" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G20" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H20" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>20.0</v>
+        <v>29.0</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="3">
-        <v>3044102.0</v>
+        <v>32</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="F21" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="H21" s="2">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1">
-        <v>21.0</v>
+        <v>31.0</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="3">
-        <v>3044636.0</v>
+        <v>32</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="F22" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G22" s="2">
-        <v>39.0</v>
+        <v>1.0</v>
       </c>
       <c r="H22" s="2">
-        <v>39.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <v>22.0</v>
+        <v>32.0</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="E23" s="3">
-        <v>3047293.0</v>
+        <v>801733.0</v>
       </c>
       <c r="F23" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G23" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H23" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>23.0</v>
+        <v>35.0</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="3">
-        <v>3047028.0</v>
+        <v>32</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="F24" s="6" t="b">
         <v>1</v>
@@ -1424,45 +1424,45 @@
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <v>24.0</v>
+        <v>36.0</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="3">
-        <v>3022276.0</v>
+        <v>32</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="F25" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G25" s="2">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
       <c r="H25" s="2">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1">
-        <v>25.0</v>
+        <v>37.0</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="3">
-        <v>3030161.0</v>
+        <v>32</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="F26" s="6" t="b">
         <v>1</v>
@@ -1476,71 +1476,71 @@
     </row>
     <row r="27">
       <c r="A27" s="1">
-        <v>26.0</v>
+        <v>39.0</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="3">
-        <v>3030213.0</v>
+        <v>32</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="F27" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G27" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H27" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1">
-        <v>27.0</v>
+        <v>40.0</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="E28" s="3">
-        <v>3036877.0</v>
+        <v>1085039.0</v>
       </c>
       <c r="F28" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G28" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H28" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1">
-        <v>28.0</v>
+        <v>41.0</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="3">
-        <v>2866310.0</v>
+        <v>57</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="F29" s="6" t="b">
         <v>1</v>
@@ -1549,50 +1549,50 @@
         <v>1.0</v>
       </c>
       <c r="H29" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1">
-        <v>29.0</v>
+        <v>43.0</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="F30" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="2">
         <v>2.0</v>
       </c>
       <c r="H30" s="2">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>65</v>
+        <v>57.0</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="F31" s="6" t="b">
         <v>1</v>
@@ -1601,24 +1601,24 @@
         <v>1.0</v>
       </c>
       <c r="H31" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>67</v>
+        <v>58.0</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="F32" s="6" t="b">
         <v>1</v>
@@ -1627,53 +1627,53 @@
         <v>1.0</v>
       </c>
       <c r="H32" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1">
-        <v>32.0</v>
+        <v>44.0</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" s="3">
-        <v>801733.0</v>
+        <v>60</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="F33" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G33" s="2">
-        <v>1.0</v>
+        <v>30.0</v>
       </c>
       <c r="H33" s="2">
-        <v>1.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1">
-        <v>33.0</v>
+        <v>45.0</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>71</v>
+        <v>35</v>
+      </c>
+      <c r="E34" s="8">
+        <v>1681389.0</v>
       </c>
       <c r="F34" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="2">
         <v>1.0</v>
@@ -1684,45 +1684,45 @@
     </row>
     <row r="35">
       <c r="A35" s="1">
-        <v>34.0</v>
+        <v>46.0</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>74</v>
+        <v>35</v>
+      </c>
+      <c r="E35" s="8">
+        <v>1668247.0</v>
       </c>
       <c r="F35" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G35" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H35" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1">
-        <v>35.0</v>
+        <v>47.0</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>76</v>
+        <v>35</v>
+      </c>
+      <c r="E36" s="8">
+        <v>1669848.0</v>
       </c>
       <c r="F36" s="6" t="b">
         <v>1</v>
@@ -1736,71 +1736,71 @@
     </row>
     <row r="37">
       <c r="A37" s="1">
-        <v>36.0</v>
+        <v>48.0</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>78</v>
+        <v>35</v>
+      </c>
+      <c r="E37" s="8">
+        <v>1668124.0</v>
       </c>
       <c r="F37" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="2">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="H37" s="2">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1">
-        <v>37.0</v>
+        <v>49.0</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>80</v>
+        <v>35</v>
+      </c>
+      <c r="E38" s="8">
+        <v>1669628.0</v>
       </c>
       <c r="F38" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G38" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H38" s="2">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1">
-        <v>38.0</v>
+        <v>50.0</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>83</v>
+        <v>65</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="F39" s="6" t="b">
         <v>1</v>
@@ -1809,50 +1809,50 @@
         <v>1.0</v>
       </c>
       <c r="H39" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1">
-        <v>39.0</v>
+        <v>51.0</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>85</v>
+        <v>35</v>
+      </c>
+      <c r="E40" s="8">
+        <v>1415943.0</v>
       </c>
       <c r="F40" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" s="2">
         <v>1.0</v>
       </c>
       <c r="H40" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1">
-        <v>40.0</v>
+        <v>52.0</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="3">
-        <v>1085039.0</v>
+        <v>32</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="F41" s="6" t="b">
         <v>1</v>
@@ -1866,123 +1866,123 @@
     </row>
     <row r="42">
       <c r="A42" s="1">
-        <v>41.0</v>
+        <v>53.0</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>88</v>
+        <v>35</v>
+      </c>
+      <c r="E42" s="8">
+        <v>1683002.0</v>
       </c>
       <c r="F42" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="2">
         <v>1.0</v>
       </c>
       <c r="H42" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1">
-        <v>42.0</v>
+        <v>54.0</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>90</v>
+        <v>65</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="F43" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G43" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H43" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1">
-        <v>43.0</v>
+        <v>55.0</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>92</v>
+        <v>65</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F44" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G44" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H44" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1">
-        <v>44.0</v>
+        <v>56.0</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>95</v>
+        <v>35</v>
+      </c>
+      <c r="E45" s="8">
+        <v>1520372.0</v>
       </c>
       <c r="F45" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" s="2">
-        <v>30.0</v>
+        <v>1.0</v>
       </c>
       <c r="H45" s="2">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1">
-        <v>45.0</v>
+        <v>2.0</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E46" s="8">
-        <v>1681389.0</v>
+        <v>87</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="F46" s="6" t="b">
         <v>1</v>
@@ -1996,45 +1996,45 @@
     </row>
     <row r="47">
       <c r="A47" s="1">
-        <v>46.0</v>
+        <v>13.0</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E47" s="8">
-        <v>1668247.0</v>
+        <v>32</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="F47" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G47" s="2">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H47" s="2">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1">
-        <v>47.0</v>
+        <v>14.0</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E48" s="8">
-        <v>1669848.0</v>
+        <v>32</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="F48" s="6" t="b">
         <v>1</v>
@@ -2048,149 +2048,149 @@
     </row>
     <row r="49">
       <c r="A49" s="1">
-        <v>48.0</v>
+        <v>15.0</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E49" s="8">
-        <v>1668124.0</v>
-      </c>
       <c r="F49" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G49" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H49" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1">
-        <v>49.0</v>
+        <v>16.0</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E50" s="8">
-        <v>1669628.0</v>
+        <v>32</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="F50" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H50" s="2">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1">
-        <v>50.0</v>
+        <v>17.0</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>103</v>
+        <v>86</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F51" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="2">
         <v>1.0</v>
       </c>
       <c r="H51" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1">
-        <v>51.0</v>
+        <v>18.0</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E52" s="8">
-        <v>1415943.0</v>
+        <v>32</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="F52" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" s="2">
         <v>1.0</v>
       </c>
       <c r="H52" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1">
-        <v>52.0</v>
+        <v>19.0</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>106</v>
+        <v>32</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="F53" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G53" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H53" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1">
-        <v>53.0</v>
+        <v>30.0</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E54" s="8">
-        <v>1683002.0</v>
+        <v>32</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="F54" s="6" t="b">
         <v>1</v>
@@ -2204,19 +2204,19 @@
     </row>
     <row r="55">
       <c r="A55" s="1">
-        <v>54.0</v>
+        <v>33.0</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>110</v>
+        <v>86</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="F55" s="6" t="b">
         <v>1</v>
@@ -2230,19 +2230,19 @@
     </row>
     <row r="56">
       <c r="A56" s="1">
-        <v>55.0</v>
+        <v>34.0</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>112</v>
+        <v>86</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="F56" s="6" t="b">
         <v>1</v>
@@ -2256,97 +2256,97 @@
     </row>
     <row r="57">
       <c r="A57" s="1">
-        <v>56.0</v>
+        <v>38.0</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E57" s="8">
-        <v>1520372.0</v>
+        <v>57</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="F57" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="2">
         <v>1.0</v>
       </c>
       <c r="H57" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1">
-        <v>57.0</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>114</v>
+        <v>42.0</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>92</v>
+        <v>32</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="F58" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H58" s="2">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1">
-        <v>58.0</v>
+        <v>76.0</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>115</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="F59" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="2">
         <v>1.0</v>
       </c>
       <c r="H59" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1">
-        <v>59.0</v>
+        <v>77.0</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>115</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F60" s="6" t="b">
         <v>1</v>
@@ -2360,16 +2360,16 @@
     </row>
     <row r="61">
       <c r="A61" s="1">
-        <v>60.0</v>
+        <v>78.0</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>120</v>
@@ -2386,19 +2386,19 @@
     </row>
     <row r="62">
       <c r="A62" s="1">
-        <v>61.0</v>
+        <v>1.0</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>41</v>
+        <v>121</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="F62" s="6" t="b">
         <v>1</v>
@@ -2412,19 +2412,19 @@
     </row>
     <row r="63">
       <c r="A63" s="1">
-        <v>62.0</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>51</v>
+        <v>79.0</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F63" s="6" t="b">
         <v>1</v>
@@ -2438,19 +2438,19 @@
     </row>
     <row r="64">
       <c r="A64" s="1">
-        <v>63.0</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>41</v>
+        <v>80.0</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F64" s="6" t="b">
         <v>1</v>
@@ -2464,22 +2464,22 @@
     </row>
     <row r="65">
       <c r="A65" s="1">
-        <v>64.0</v>
+        <v>81.0</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F65" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" s="2">
         <v>1.0</v>
@@ -2490,19 +2490,19 @@
     </row>
     <row r="66">
       <c r="A66" s="1">
-        <v>65.0</v>
+        <v>82.0</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="F66" s="6" t="b">
         <v>1</v>
@@ -2516,22 +2516,22 @@
     </row>
     <row r="67">
       <c r="A67" s="1">
-        <v>66.0</v>
+        <v>83.0</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F67" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67" s="2">
         <v>1.0</v>
@@ -2542,19 +2542,19 @@
     </row>
     <row r="68">
       <c r="A68" s="1">
-        <v>67.0</v>
+        <v>59.0</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>129</v>
+        <v>63</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="F68" s="6" t="b">
         <v>1</v>
@@ -2568,45 +2568,45 @@
     </row>
     <row r="69">
       <c r="A69" s="1">
-        <v>68.0</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>53</v>
+        <v>60.0</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>54</v>
+        <v>136</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="F69" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G69" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H69" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1">
-        <v>69.0</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>132</v>
+        <v>61.0</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="F70" s="6" t="b">
         <v>1</v>
@@ -2620,19 +2620,19 @@
     </row>
     <row r="71">
       <c r="A71" s="1">
-        <v>70.0</v>
+        <v>62.0</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="F71" s="6" t="b">
         <v>1</v>
@@ -2646,71 +2646,71 @@
     </row>
     <row r="72">
       <c r="A72" s="1">
-        <v>71.0</v>
+        <v>63.0</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F72" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G72" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H72" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1">
-        <v>72.0</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>47</v>
+        <v>64.0</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>48</v>
+        <v>73</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="F73" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G73" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H73" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1">
-        <v>73.0</v>
+        <v>65.0</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="D74" s="2" t="s">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="F74" s="6" t="b">
         <v>1</v>
@@ -2724,19 +2724,19 @@
     </row>
     <row r="75">
       <c r="A75" s="1">
-        <v>74.0</v>
+        <v>66.0</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>135</v>
+        <v>80</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F75" s="6" t="b">
         <v>1</v>
@@ -2750,19 +2750,19 @@
     </row>
     <row r="76">
       <c r="A76" s="1">
-        <v>75.0</v>
+        <v>67.0</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="F76" s="6" t="b">
         <v>1</v>
@@ -2776,45 +2776,45 @@
     </row>
     <row r="77">
       <c r="A77" s="1">
-        <v>76.0</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>141</v>
+        <v>68.0</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>142</v>
+        <v>32</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="F77" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G77" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H77" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1">
-        <v>77.0</v>
+        <v>69.0</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>144</v>
+        <v>32</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="F78" s="6" t="b">
         <v>1</v>
@@ -2828,19 +2828,19 @@
     </row>
     <row r="79">
       <c r="A79" s="1">
-        <v>78.0</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>145</v>
+        <v>70.0</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>146</v>
+        <v>32</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="F79" s="6" t="b">
         <v>1</v>
@@ -2854,68 +2854,68 @@
     </row>
     <row r="80">
       <c r="A80" s="1">
-        <v>79.0</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>147</v>
+        <v>71.0</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>148</v>
+        <v>32</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="F80" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G80" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H80" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1">
-        <v>80.0</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>149</v>
+        <v>72.0</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>150</v>
+        <v>32</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="F81" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H81" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1">
-        <v>81.0</v>
+        <v>73.0</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>151</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>152</v>
@@ -2932,22 +2932,22 @@
     </row>
     <row r="83">
       <c r="A83" s="1">
-        <v>82.0</v>
+        <v>74.0</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>153</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F83" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83" s="2">
         <v>1.0</v>
@@ -2958,16 +2958,16 @@
     </row>
     <row r="84">
       <c r="A84" s="1">
-        <v>83.0</v>
+        <v>75.0</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>155</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>156</v>

</xml_diff>